<commit_message>
Add a new features
Enable appending of new data to previously scraped data for scheduling purpose
</commit_message>
<xml_diff>
--- a/stock_index_sectoral.xlsx
+++ b/stock_index_sectoral.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>DTCreate</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>LastScraped</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -487,25 +492,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2046.37</v>
+        <v>1946.869</v>
       </c>
       <c r="C2" t="n">
-        <v>2062.614</v>
+        <v>2013.924</v>
       </c>
       <c r="D2" t="n">
-        <v>2046.37</v>
+        <v>1946.869</v>
       </c>
       <c r="E2" t="n">
-        <v>2060.846</v>
+        <v>2013.924</v>
       </c>
       <c r="F2" t="n">
-        <v>14.48</v>
+        <v>67.06</v>
       </c>
       <c r="G2" t="n">
-        <v>0.71</v>
+        <v>3.44</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="3">
@@ -515,25 +523,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1177.599</v>
+        <v>1106.896</v>
       </c>
       <c r="C3" t="n">
-        <v>1187.853</v>
+        <v>1127.315</v>
       </c>
       <c r="D3" t="n">
-        <v>1177.599</v>
+        <v>1106.896</v>
       </c>
       <c r="E3" t="n">
-        <v>1178.828</v>
+        <v>1125.892</v>
       </c>
       <c r="F3" t="n">
-        <v>1.23</v>
+        <v>19</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1</v>
+        <v>1.72</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="4">
@@ -543,25 +554,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1164.917</v>
+        <v>1130.866</v>
       </c>
       <c r="C4" t="n">
-        <v>1180.671</v>
+        <v>1151.763</v>
       </c>
       <c r="D4" t="n">
-        <v>1164.917</v>
+        <v>1130.866</v>
       </c>
       <c r="E4" t="n">
-        <v>1176.184</v>
+        <v>1151.763</v>
       </c>
       <c r="F4" t="n">
-        <v>11.27</v>
+        <v>20.9</v>
       </c>
       <c r="G4" t="n">
-        <v>0.97</v>
+        <v>1.85</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="5">
@@ -571,25 +585,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>732.02</v>
+        <v>710.956</v>
       </c>
       <c r="C5" t="n">
-        <v>734.7380000000001</v>
+        <v>724.1420000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>728.4640000000001</v>
+        <v>710.956</v>
       </c>
       <c r="E5" t="n">
-        <v>728.898</v>
+        <v>717.836</v>
       </c>
       <c r="F5" t="n">
-        <v>-3.12</v>
+        <v>6.88</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.43</v>
+        <v>0.97</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="6">
@@ -599,25 +616,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>833.2910000000001</v>
+        <v>789.999</v>
       </c>
       <c r="C6" t="n">
-        <v>835.335</v>
+        <v>801.053</v>
       </c>
       <c r="D6" t="n">
-        <v>829.76</v>
+        <v>789.73</v>
       </c>
       <c r="E6" t="n">
-        <v>834.4160000000001</v>
+        <v>795.524</v>
       </c>
       <c r="F6" t="n">
-        <v>1.13</v>
+        <v>5.53</v>
       </c>
       <c r="G6" t="n">
-        <v>0.14</v>
+        <v>0.7</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="7">
@@ -627,25 +647,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1529.897</v>
+        <v>1534.586</v>
       </c>
       <c r="C7" t="n">
-        <v>1553.551</v>
+        <v>1562.97</v>
       </c>
       <c r="D7" t="n">
-        <v>1528.28</v>
+        <v>1534.586</v>
       </c>
       <c r="E7" t="n">
-        <v>1547.101</v>
+        <v>1562.97</v>
       </c>
       <c r="F7" t="n">
-        <v>17.2</v>
+        <v>28.38</v>
       </c>
       <c r="G7" t="n">
-        <v>1.13</v>
+        <v>1.85</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="8">
@@ -655,25 +678,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1398.116</v>
+        <v>1339.677</v>
       </c>
       <c r="C8" t="n">
-        <v>1409.304</v>
+        <v>1365.554</v>
       </c>
       <c r="D8" t="n">
-        <v>1398.116</v>
+        <v>1339.677</v>
       </c>
       <c r="E8" t="n">
-        <v>1403.41</v>
+        <v>1364.895</v>
       </c>
       <c r="F8" t="n">
-        <v>5.29</v>
+        <v>25.22</v>
       </c>
       <c r="G8" t="n">
-        <v>0.38</v>
+        <v>1.88</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="9">
@@ -683,25 +709,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>685.092</v>
+        <v>664.515</v>
       </c>
       <c r="C9" t="n">
-        <v>686.932</v>
+        <v>667.583</v>
       </c>
       <c r="D9" t="n">
-        <v>682.652</v>
+        <v>663.032</v>
       </c>
       <c r="E9" t="n">
-        <v>684.302</v>
+        <v>664.827</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.79</v>
+        <v>0.31</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.12</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="10">
@@ -711,25 +740,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5423.281</v>
+        <v>5028.5</v>
       </c>
       <c r="C10" t="n">
-        <v>5462.393</v>
+        <v>5130.004</v>
       </c>
       <c r="D10" t="n">
-        <v>5400.828</v>
+        <v>4971.998</v>
       </c>
       <c r="E10" t="n">
-        <v>5430.508</v>
+        <v>5023.903</v>
       </c>
       <c r="F10" t="n">
-        <v>7.23</v>
+        <v>-4.6</v>
       </c>
       <c r="G10" t="n">
-        <v>0.13</v>
+        <v>-0.09</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="11">
@@ -739,25 +771,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>835.374</v>
+        <v>795.948</v>
       </c>
       <c r="C11" t="n">
-        <v>842.989</v>
+        <v>811.947</v>
       </c>
       <c r="D11" t="n">
-        <v>833.496</v>
+        <v>795.948</v>
       </c>
       <c r="E11" t="n">
-        <v>836.4</v>
+        <v>808.279</v>
       </c>
       <c r="F11" t="n">
-        <v>1.03</v>
+        <v>12.33</v>
       </c>
       <c r="G11" t="n">
-        <v>0.12</v>
+        <v>1.55</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
     <row r="12">
@@ -767,25 +802,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1811.626</v>
+        <v>1695.772</v>
       </c>
       <c r="C12" t="n">
-        <v>1846.16</v>
+        <v>1744.592</v>
       </c>
       <c r="D12" t="n">
-        <v>1811.626</v>
+        <v>1695.772</v>
       </c>
       <c r="E12" t="n">
-        <v>1841.278</v>
+        <v>1744.592</v>
       </c>
       <c r="F12" t="n">
-        <v>29.65</v>
+        <v>48.82</v>
       </c>
       <c r="G12" t="n">
-        <v>1.64</v>
+        <v>2.88</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>45004.83881353009</v>
       </c>
     </row>
   </sheetData>
@@ -799,7 +837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -845,7 +883,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>DtCreate</t>
+          <t>DTCreate</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>LastScraped</t>
         </is>
       </c>
     </row>
@@ -856,25 +899,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6776.37</v>
+        <v>6565.728</v>
       </c>
       <c r="C2" t="n">
-        <v>6824.664</v>
+        <v>6683.094</v>
       </c>
       <c r="D2" t="n">
-        <v>6776.37</v>
+        <v>6565.728</v>
       </c>
       <c r="E2" t="n">
-        <v>6799.795</v>
+        <v>6678.237</v>
       </c>
       <c r="F2" t="n">
-        <v>23.43</v>
+        <v>112.51</v>
       </c>
       <c r="G2" t="n">
-        <v>0.35</v>
+        <v>1.71</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="3">
@@ -884,25 +930,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1871.653</v>
+        <v>1812.606</v>
       </c>
       <c r="C3" t="n">
-        <v>1885.474</v>
+        <v>1847.457</v>
       </c>
       <c r="D3" t="n">
-        <v>1871.653</v>
+        <v>1812.606</v>
       </c>
       <c r="E3" t="n">
-        <v>1878.498</v>
+        <v>1845.111</v>
       </c>
       <c r="F3" t="n">
-        <v>6.85</v>
+        <v>32.51</v>
       </c>
       <c r="G3" t="n">
-        <v>0.37</v>
+        <v>1.79</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="4">
@@ -912,25 +961,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1618.408</v>
+        <v>1568.22</v>
       </c>
       <c r="C4" t="n">
-        <v>1627.412</v>
+        <v>1583.489</v>
       </c>
       <c r="D4" t="n">
-        <v>1618.408</v>
+        <v>1568.22</v>
       </c>
       <c r="E4" t="n">
-        <v>1623.033</v>
+        <v>1583.489</v>
       </c>
       <c r="F4" t="n">
-        <v>4.63</v>
+        <v>15.27</v>
       </c>
       <c r="G4" t="n">
-        <v>0.29</v>
+        <v>0.97</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="5">
@@ -940,25 +992,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1159.914</v>
+        <v>1118.593</v>
       </c>
       <c r="C5" t="n">
-        <v>1171.197</v>
+        <v>1140.513</v>
       </c>
       <c r="D5" t="n">
-        <v>1159.914</v>
+        <v>1118.593</v>
       </c>
       <c r="E5" t="n">
-        <v>1165.446</v>
+        <v>1138.755</v>
       </c>
       <c r="F5" t="n">
-        <v>5.53</v>
+        <v>20.16</v>
       </c>
       <c r="G5" t="n">
-        <v>0.48</v>
+        <v>1.8</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="6">
@@ -968,25 +1023,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1133.343</v>
+        <v>1096.891</v>
       </c>
       <c r="C6" t="n">
-        <v>1149.072</v>
+        <v>1123.753</v>
       </c>
       <c r="D6" t="n">
-        <v>1138.95</v>
+        <v>1104.197</v>
       </c>
       <c r="E6" t="n">
-        <v>1142.632</v>
+        <v>1118.152</v>
       </c>
       <c r="F6" t="n">
-        <v>9.289999999999999</v>
+        <v>21.26</v>
       </c>
       <c r="G6" t="n">
-        <v>0.82</v>
+        <v>1.94</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="7">
@@ -996,25 +1054,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>939.035</v>
+        <v>907.501</v>
       </c>
       <c r="C7" t="n">
-        <v>948.5170000000001</v>
+        <v>926.465</v>
       </c>
       <c r="D7" t="n">
-        <v>939.035</v>
+        <v>907.501</v>
       </c>
       <c r="E7" t="n">
-        <v>942.885</v>
+        <v>924.254</v>
       </c>
       <c r="F7" t="n">
-        <v>3.85</v>
+        <v>16.75</v>
       </c>
       <c r="G7" t="n">
-        <v>0.41</v>
+        <v>1.85</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="8">
@@ -1024,25 +1085,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>580.975</v>
+        <v>566.974</v>
       </c>
       <c r="C8" t="n">
-        <v>587.557</v>
+        <v>579.335</v>
       </c>
       <c r="D8" t="n">
-        <v>580.975</v>
+        <v>566.974</v>
       </c>
       <c r="E8" t="n">
-        <v>583.955</v>
+        <v>577.761</v>
       </c>
       <c r="F8" t="n">
-        <v>2.98</v>
+        <v>10.79</v>
       </c>
       <c r="G8" t="n">
-        <v>0.51</v>
+        <v>1.9</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="9">
@@ -1052,25 +1116,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>562.994</v>
+        <v>546.038</v>
       </c>
       <c r="C9" t="n">
-        <v>567.9880000000001</v>
+        <v>560.2</v>
       </c>
       <c r="D9" t="n">
-        <v>562.994</v>
+        <v>546.038</v>
       </c>
       <c r="E9" t="n">
-        <v>564.851</v>
+        <v>560.2</v>
       </c>
       <c r="F9" t="n">
-        <v>1.86</v>
+        <v>14.16</v>
       </c>
       <c r="G9" t="n">
-        <v>0.33</v>
+        <v>2.59</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="10">
@@ -1080,25 +1147,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>559.386</v>
+        <v>547.47</v>
       </c>
       <c r="C10" t="n">
-        <v>566.042</v>
+        <v>559.034</v>
       </c>
       <c r="D10" t="n">
-        <v>559.386</v>
+        <v>547.47</v>
       </c>
       <c r="E10" t="n">
-        <v>563.296</v>
+        <v>558.395</v>
       </c>
       <c r="F10" t="n">
-        <v>3.91</v>
+        <v>10.93</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="11">
@@ -1108,25 +1178,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>489.257</v>
+        <v>473.932</v>
       </c>
       <c r="C11" t="n">
-        <v>494.31</v>
+        <v>483.53</v>
       </c>
       <c r="D11" t="n">
-        <v>489.257</v>
+        <v>473.932</v>
       </c>
       <c r="E11" t="n">
-        <v>491.287</v>
+        <v>482.45</v>
       </c>
       <c r="F11" t="n">
-        <v>2.03</v>
+        <v>8.52</v>
       </c>
       <c r="G11" t="n">
-        <v>0.42</v>
+        <v>1.8</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="12">
@@ -1136,25 +1209,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>485.108</v>
+        <v>472.024</v>
       </c>
       <c r="C12" t="n">
-        <v>490.286</v>
+        <v>482.645</v>
       </c>
       <c r="D12" t="n">
-        <v>485.108</v>
+        <v>472.024</v>
       </c>
       <c r="E12" t="n">
-        <v>487.432</v>
+        <v>481.397</v>
       </c>
       <c r="F12" t="n">
-        <v>2.32</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="G12" t="n">
-        <v>0.48</v>
+        <v>1.99</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="13">
@@ -1164,25 +1240,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>418.746</v>
+        <v>410.189</v>
       </c>
       <c r="C13" t="n">
-        <v>423.85</v>
+        <v>418.708</v>
       </c>
       <c r="D13" t="n">
-        <v>418.746</v>
+        <v>410.189</v>
       </c>
       <c r="E13" t="n">
-        <v>421.64</v>
+        <v>417.357</v>
       </c>
       <c r="F13" t="n">
-        <v>2.89</v>
+        <v>7.17</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6899999999999999</v>
+        <v>1.75</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="14">
@@ -1192,81 +1271,90 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>400.148</v>
+        <v>386.326</v>
       </c>
       <c r="C14" t="n">
-        <v>405.386</v>
+        <v>395.756</v>
       </c>
       <c r="D14" t="n">
-        <v>400.148</v>
+        <v>386.326</v>
       </c>
       <c r="E14" t="n">
-        <v>403.921</v>
+        <v>395.756</v>
       </c>
       <c r="F14" t="n">
-        <v>3.77</v>
+        <v>9.43</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9399999999999999</v>
+        <v>2.44</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IDXSMC-LIQ</t>
+          <t>MNC36</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>363.702</v>
+        <v>344.052</v>
       </c>
       <c r="C15" t="n">
-        <v>366.966</v>
+        <v>351.416</v>
       </c>
       <c r="D15" t="n">
-        <v>363.702</v>
+        <v>344.052</v>
       </c>
       <c r="E15" t="n">
-        <v>366.561</v>
+        <v>350.698</v>
       </c>
       <c r="F15" t="n">
-        <v>2.86</v>
+        <v>6.65</v>
       </c>
       <c r="G15" t="n">
-        <v>0.79</v>
+        <v>1.93</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MNC36</t>
+          <t>IDXSMC-LIQ</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>352.854</v>
+        <v>340.561</v>
       </c>
       <c r="C16" t="n">
-        <v>356.837</v>
+        <v>346.613</v>
       </c>
       <c r="D16" t="n">
-        <v>352.854</v>
+        <v>340.561</v>
       </c>
       <c r="E16" t="n">
-        <v>354.896</v>
+        <v>346.613</v>
       </c>
       <c r="F16" t="n">
-        <v>2.04</v>
+        <v>6.05</v>
       </c>
       <c r="G16" t="n">
-        <v>0.58</v>
+        <v>1.78</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="17">
@@ -1276,25 +1364,28 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>341.985</v>
+        <v>322.708</v>
       </c>
       <c r="C17" t="n">
-        <v>343.931</v>
+        <v>327.943</v>
       </c>
       <c r="D17" t="n">
-        <v>341.985</v>
+        <v>322.708</v>
       </c>
       <c r="E17" t="n">
-        <v>343.441</v>
+        <v>327.943</v>
       </c>
       <c r="F17" t="n">
-        <v>1.46</v>
+        <v>5.24</v>
       </c>
       <c r="G17" t="n">
-        <v>0.43</v>
+        <v>1.62</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="18">
@@ -1304,25 +1395,28 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>309.469</v>
+        <v>296.667</v>
       </c>
       <c r="C18" t="n">
-        <v>313.82</v>
+        <v>303.729</v>
       </c>
       <c r="D18" t="n">
-        <v>309.469</v>
+        <v>296.667</v>
       </c>
       <c r="E18" t="n">
-        <v>312.25</v>
+        <v>303.359</v>
       </c>
       <c r="F18" t="n">
-        <v>2.78</v>
+        <v>6.69</v>
       </c>
       <c r="G18" t="n">
-        <v>0.9</v>
+        <v>2.26</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="19">
@@ -1332,25 +1426,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>258.925</v>
+        <v>243.495</v>
       </c>
       <c r="C19" t="n">
-        <v>259.985</v>
+        <v>247.844</v>
       </c>
       <c r="D19" t="n">
-        <v>258.444</v>
+        <v>243.495</v>
       </c>
       <c r="E19" t="n">
-        <v>258.509</v>
+        <v>247.844</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.42</v>
+        <v>4.35</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.16</v>
+        <v>1.79</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="20">
@@ -1360,25 +1457,28 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>207.497</v>
+        <v>201.946</v>
       </c>
       <c r="C20" t="n">
-        <v>208.538</v>
+        <v>205.965</v>
       </c>
       <c r="D20" t="n">
-        <v>207.497</v>
+        <v>201.946</v>
       </c>
       <c r="E20" t="n">
-        <v>208.041</v>
+        <v>205.965</v>
       </c>
       <c r="F20" t="n">
-        <v>0.54</v>
+        <v>4.02</v>
       </c>
       <c r="G20" t="n">
-        <v>0.26</v>
+        <v>1.99</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="21">
@@ -1388,25 +1488,28 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>205.239</v>
+        <v>200.548</v>
       </c>
       <c r="C21" t="n">
-        <v>207.858</v>
+        <v>204.763</v>
       </c>
       <c r="D21" t="n">
-        <v>205.239</v>
+        <v>200.548</v>
       </c>
       <c r="E21" t="n">
-        <v>206.535</v>
+        <v>203.966</v>
       </c>
       <c r="F21" t="n">
-        <v>1.3</v>
+        <v>3.42</v>
       </c>
       <c r="G21" t="n">
-        <v>0.63</v>
+        <v>1.7</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="22">
@@ -1416,25 +1519,28 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>191.125</v>
+        <v>184.287</v>
       </c>
       <c r="C22" t="n">
-        <v>192.437</v>
+        <v>188.627</v>
       </c>
       <c r="D22" t="n">
-        <v>191.125</v>
+        <v>184.287</v>
       </c>
       <c r="E22" t="n">
-        <v>191.57</v>
+        <v>188.627</v>
       </c>
       <c r="F22" t="n">
-        <v>0.45</v>
+        <v>4.34</v>
       </c>
       <c r="G22" t="n">
-        <v>0.23</v>
+        <v>2.36</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="23">
@@ -1444,25 +1550,28 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>160.168</v>
+        <v>156.148</v>
       </c>
       <c r="C23" t="n">
-        <v>161.737</v>
+        <v>159.714</v>
       </c>
       <c r="D23" t="n">
-        <v>160.168</v>
+        <v>156.148</v>
       </c>
       <c r="E23" t="n">
-        <v>160.982</v>
+        <v>159.502</v>
       </c>
       <c r="F23" t="n">
-        <v>0.8100000000000001</v>
+        <v>3.35</v>
       </c>
       <c r="G23" t="n">
-        <v>0.51</v>
+        <v>2.15</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="24">
@@ -1472,81 +1581,90 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>151.581</v>
+        <v>147.911</v>
       </c>
       <c r="C24" t="n">
-        <v>153.289</v>
+        <v>151.038</v>
       </c>
       <c r="D24" t="n">
-        <v>152.169</v>
+        <v>148.905</v>
       </c>
       <c r="E24" t="n">
-        <v>152.353</v>
+        <v>150.594</v>
       </c>
       <c r="F24" t="n">
-        <v>0.77</v>
+        <v>2.68</v>
       </c>
       <c r="G24" t="n">
-        <v>0.51</v>
+        <v>1.81</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>IDXV30</t>
+          <t>IDXESGL</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>141.666</v>
+        <v>135.777</v>
       </c>
       <c r="C25" t="n">
-        <v>143.428</v>
+        <v>138.308</v>
       </c>
       <c r="D25" t="n">
-        <v>141.666</v>
+        <v>135.777</v>
       </c>
       <c r="E25" t="n">
-        <v>142.936</v>
+        <v>137.526</v>
       </c>
       <c r="F25" t="n">
-        <v>1.27</v>
+        <v>1.75</v>
       </c>
       <c r="G25" t="n">
-        <v>0.9</v>
+        <v>1.29</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IDXESGL</t>
+          <t>IDXV30</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>139.733</v>
+        <v>134.321</v>
       </c>
       <c r="C26" t="n">
-        <v>141.371</v>
+        <v>138.113</v>
       </c>
       <c r="D26" t="n">
-        <v>139.733</v>
+        <v>134.321</v>
       </c>
       <c r="E26" t="n">
-        <v>140.656</v>
+        <v>138.113</v>
       </c>
       <c r="F26" t="n">
-        <v>0.92</v>
+        <v>3.79</v>
       </c>
       <c r="G26" t="n">
-        <v>0.66</v>
+        <v>2.82</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="27">
@@ -1556,25 +1674,28 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>136.164</v>
+        <v>133.076</v>
       </c>
       <c r="C27" t="n">
-        <v>137.674</v>
+        <v>135.89</v>
       </c>
       <c r="D27" t="n">
-        <v>136.164</v>
+        <v>133.076</v>
       </c>
       <c r="E27" t="n">
-        <v>136.949</v>
+        <v>135.434</v>
       </c>
       <c r="F27" t="n">
-        <v>0.79</v>
+        <v>2.36</v>
       </c>
       <c r="G27" t="n">
-        <v>0.58</v>
+        <v>1.77</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="28">
@@ -1584,25 +1705,28 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>136.093</v>
+        <v>132.428</v>
       </c>
       <c r="C28" t="n">
-        <v>137.619</v>
+        <v>135.167</v>
       </c>
       <c r="D28" t="n">
-        <v>136.093</v>
+        <v>132.428</v>
       </c>
       <c r="E28" t="n">
-        <v>136.777</v>
+        <v>134.709</v>
       </c>
       <c r="F28" t="n">
-        <v>0.68</v>
+        <v>2.28</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5</v>
+        <v>1.72</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="29">
@@ -1612,25 +1736,28 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>130.997</v>
+        <v>126.352</v>
       </c>
       <c r="C29" t="n">
-        <v>132.287</v>
+        <v>128.828</v>
       </c>
       <c r="D29" t="n">
-        <v>130.997</v>
+        <v>126.352</v>
       </c>
       <c r="E29" t="n">
-        <v>131.624</v>
+        <v>128.631</v>
       </c>
       <c r="F29" t="n">
-        <v>0.63</v>
+        <v>2.28</v>
       </c>
       <c r="G29" t="n">
-        <v>0.48</v>
+        <v>1.8</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="30">
@@ -1640,25 +1767,28 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>128.674</v>
+        <v>126.223</v>
       </c>
       <c r="C30" t="n">
-        <v>130.476</v>
+        <v>128.543</v>
       </c>
       <c r="D30" t="n">
-        <v>128.674</v>
+        <v>126.223</v>
       </c>
       <c r="E30" t="n">
-        <v>129.739</v>
+        <v>127.88</v>
       </c>
       <c r="F30" t="n">
-        <v>1.07</v>
+        <v>1.66</v>
       </c>
       <c r="G30" t="n">
-        <v>0.83</v>
+        <v>1.31</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="31">
@@ -1668,25 +1798,28 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>104.857</v>
+        <v>102.358</v>
       </c>
       <c r="C31" t="n">
-        <v>105.867</v>
+        <v>105.145</v>
       </c>
       <c r="D31" t="n">
-        <v>104.857</v>
+        <v>102.358</v>
       </c>
       <c r="E31" t="n">
-        <v>105.328</v>
+        <v>105.145</v>
       </c>
       <c r="F31" t="n">
-        <v>0.47</v>
+        <v>2.79</v>
       </c>
       <c r="G31" t="n">
-        <v>0.45</v>
+        <v>2.72</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
     <row r="32">
@@ -1696,25 +1829,28 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>91.40600000000001</v>
+        <v>85.84</v>
       </c>
       <c r="C32" t="n">
-        <v>92.527</v>
+        <v>88.17100000000001</v>
       </c>
       <c r="D32" t="n">
-        <v>91.40600000000001</v>
+        <v>85.84</v>
       </c>
       <c r="E32" t="n">
-        <v>92.205</v>
+        <v>88.17100000000001</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8</v>
+        <v>2.33</v>
       </c>
       <c r="G32" t="n">
-        <v>0.87</v>
+        <v>2.72</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>44994</v>
+        <v>45002</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>45004.94032903935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>